<commit_message>
Normalize URNs before looking for duplicates in imports
</commit_message>
<xml_diff>
--- a/media/test_imports/duplicate_urn.xlsx
+++ b/media/test_imports/duplicate_urn.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="8">
   <si>
     <t>URN:Tel</t>
   </si>
@@ -19,13 +19,22 @@
     <t>name</t>
   </si>
   <si>
+    <t>+250788382382</t>
+  </si>
+  <si>
     <t>Eric Newcomer</t>
   </si>
   <si>
-    <t>NIC POTTIER</t>
+    <t>+250788383383</t>
   </si>
   <si>
-    <t>jen newcomer</t>
+    <t>Nic Pottier</t>
+  </si>
+  <si>
+    <t>(+250) 788 382382</t>
+  </si>
+  <si>
+    <t>Jen Newcomer</t>
   </si>
 </sst>
 </file>
@@ -95,7 +104,7 @@
       <alignment vertical="bottom"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
@@ -106,9 +115,6 @@
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top"/>
     </xf>
   </cellXfs>
@@ -267,13 +273,7 @@
           <a:effectLst/>
         </a:effectStyle>
         <a:effectStyle>
-          <a:effectLst>
-            <a:outerShdw sx="100000" sy="100000" kx="0" ky="0" algn="b" rotWithShape="0" blurRad="38100" dist="20000" dir="5400000">
-              <a:srgbClr val="000000">
-                <a:alpha val="38000"/>
-              </a:srgbClr>
-            </a:outerShdw>
-          </a:effectLst>
+          <a:effectLst/>
         </a:effectStyle>
       </a:effectStyleLst>
       <a:bgFillStyleLst>
@@ -372,10 +372,10 @@
             </a:solidFill>
             <a:effectLst/>
             <a:uFillTx/>
-            <a:latin typeface="Calibri"/>
-            <a:ea typeface="Calibri"/>
-            <a:cs typeface="Calibri"/>
-            <a:sym typeface="Calibri"/>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+            <a:sym typeface="Helvetica Neue"/>
           </a:defRPr>
         </a:defPPr>
         <a:lvl1pPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="1" hangingPunct="0">
@@ -630,13 +630,7 @@
           <a:prstDash val="solid"/>
           <a:round/>
         </a:ln>
-        <a:effectLst>
-          <a:outerShdw sx="100000" sy="100000" kx="0" ky="0" algn="b" rotWithShape="0" blurRad="38100" dist="20000" dir="5400000">
-            <a:srgbClr val="000000">
-              <a:alpha val="38000"/>
-            </a:srgbClr>
-          </a:outerShdw>
-        </a:effectLst>
+        <a:effectLst/>
         <a:sp3d/>
       </a:spPr>
       <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="91439" tIns="45719" rIns="91439" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="t" upright="0">
@@ -921,7 +915,7 @@
         <a:effectLst/>
         <a:sp3d/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45719" tIns="45719" rIns="45719" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="t" upright="0">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45718" tIns="45718" rIns="45718" bIns="45718" numCol="1" spcCol="38100" rtlCol="0" anchor="t" upright="0">
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -949,10 +943,10 @@
             </a:solidFill>
             <a:effectLst/>
             <a:uFillTx/>
-            <a:latin typeface="Calibri"/>
-            <a:ea typeface="Calibri"/>
-            <a:cs typeface="Calibri"/>
-            <a:sym typeface="Calibri"/>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+            <a:sym typeface="Helvetica Neue"/>
           </a:defRPr>
         </a:defPPr>
         <a:lvl1pPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="1" hangingPunct="0">
@@ -1227,33 +1221,33 @@
       <c r="E1" s="3"/>
     </row>
     <row r="2" ht="20" customHeight="1">
-      <c r="A2" s="4">
-        <v>250788382382</v>
+      <c r="A2" t="s" s="2">
+        <v>2</v>
       </c>
       <c r="B2" t="s" s="2">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C2" s="3"/>
       <c r="D2" s="3"/>
       <c r="E2" s="3"/>
     </row>
     <row r="3" ht="20" customHeight="1">
-      <c r="A3" s="4">
-        <v>250788383383</v>
+      <c r="A3" t="s" s="2">
+        <v>4</v>
       </c>
       <c r="B3" t="s" s="2">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C3" s="3"/>
       <c r="D3" s="3"/>
       <c r="E3" s="3"/>
     </row>
     <row r="4" ht="20" customHeight="1">
-      <c r="A4" s="4">
-        <v>250788382382</v>
+      <c r="A4" t="s" s="2">
+        <v>6</v>
       </c>
       <c r="B4" t="s" s="2">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="C4" s="3"/>
       <c r="D4" s="3"/>

</xml_diff>